<commit_message>
JM - added SMC in STOWINS
</commit_message>
<xml_diff>
--- a/SMDG-STOWINS-CodeList .xlsx
+++ b/SMDG-STOWINS-CodeList .xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jostf\OneDrive\Dokumente\Codelists\STOWINS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602EAC3A-0269-491B-A835-E349AA3CE252}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="22470" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STOWINS" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Changelog!$A$1:$D$18</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">STOWINS!$A$9:$F$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">STOWINS!$A$9:$F$63</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="177">
   <si>
     <t>SMDG STOWAGE Instruction code list</t>
   </si>
@@ -543,12 +549,24 @@
   </si>
   <si>
     <t>Under waterline</t>
+  </si>
+  <si>
+    <t>SMC</t>
+  </si>
+  <si>
+    <t>Smart container with IoT-Device</t>
+  </si>
+  <si>
+    <t>Smart container, care for proper stowage on means of transport</t>
+  </si>
+  <si>
+    <t>added</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -710,7 +728,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -811,6 +829,19 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -861,7 +892,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8129D86-04D9-4793-B715-DF958695C765}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8129D86-04D9-4793-B715-DF958695C765}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1151,19 +1182,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="A57" sqref="A57:XFD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1187,12 +1218,12 @@
       <c r="D1" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
     </row>
     <row r="4" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D4" s="15"/>
@@ -1203,12 +1234,12 @@
       <c r="B5" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
     </row>
     <row r="6" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="18"/>
@@ -1224,12 +1255,12 @@
       <c r="B7" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
     </row>
     <row r="9" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
@@ -2003,79 +2034,81 @@
       </c>
       <c r="F56" s="11"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="12" t="s">
+    <row r="57" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="B57" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="C57" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="D57" s="36">
+        <v>44131</v>
+      </c>
+      <c r="E57" s="37">
+        <v>44131</v>
+      </c>
+      <c r="F57" s="38"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="B57" s="12" t="s">
+      <c r="B58" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C57" s="12" t="s">
+      <c r="C58" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10">
+      <c r="D58" s="10"/>
+      <c r="E58" s="10">
         <v>41640</v>
       </c>
-      <c r="F57" s="11"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="24" t="s">
+      <c r="F58" s="11"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B58" s="25" t="s">
+      <c r="B59" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C58" s="25" t="s">
+      <c r="C59" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="D58" s="10"/>
-      <c r="E58" s="11">
+      <c r="D59" s="10"/>
+      <c r="E59" s="11">
         <v>43724</v>
       </c>
-      <c r="F58" s="11"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="12" t="s">
+      <c r="F59" s="11"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="B59" s="12" t="s">
+      <c r="B60" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C59" s="12" t="s">
+      <c r="C60" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10">
+      <c r="D60" s="10"/>
+      <c r="E60" s="10">
         <v>41640</v>
-      </c>
-      <c r="F59" s="11"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="B60" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="C60" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="D60" s="10"/>
-      <c r="E60" s="11">
-        <v>43724</v>
       </c>
       <c r="F60" s="11"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="24" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B61" s="25" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C61" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D61" s="10"/>
       <c r="E61" s="11">
@@ -2084,25 +2117,41 @@
       <c r="F61" s="11"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="12" t="s">
+      <c r="A62" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="B62" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="C62" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="D62" s="10"/>
+      <c r="E62" s="11">
+        <v>43724</v>
+      </c>
+      <c r="F62" s="11"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B62" s="12" t="s">
+      <c r="B63" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="C62" s="12" t="s">
+      <c r="C63" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10">
+      <c r="D63" s="10"/>
+      <c r="E63" s="10">
         <v>43504</v>
       </c>
-      <c r="F62" s="11"/>
+      <c r="F63" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:F62"/>
-  <sortState ref="A9:E61">
-    <sortCondition ref="A9:A61"/>
+  <autoFilter ref="A9:F63" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:E62">
+    <sortCondition ref="A9:A62"/>
   </sortState>
   <mergeCells count="3">
     <mergeCell ref="C5:F5"/>
@@ -2116,12 +2165,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2129,7 +2178,7 @@
     <col min="1" max="1" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" style="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.42578125" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="31" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
@@ -2167,11 +2216,19 @@
       </c>
       <c r="D3" s="30"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>44131</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
@@ -2300,7 +2357,7 @@
       <c r="D25" s="30"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D18"/>
+  <autoFilter ref="A1:D18" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>